<commit_message>
Atualização no EscritorExcel e finalização dos assuntos
</commit_message>
<xml_diff>
--- a/server/sisata/src/main/resources/templates/template.xlsx
+++ b/server/sisata/src/main/resources/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesley\Documents\GitHub\ProjectSisatas\server\sisata\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6408165A-EF2F-435D-BDFA-380083E3D572}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45C61C0-041E-4C47-9F3B-E699DA640DE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>E-mail</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Área</t>
-  </si>
-  <si>
-    <t>Projeto:</t>
   </si>
 </sst>
 </file>
@@ -255,19 +252,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -279,11 +272,54 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -302,48 +338,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,18 +711,18 @@
   <dimension ref="B1:X921"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="8.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" width="4" style="8" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.85546875" style="8" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.85546875" style="8" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
@@ -757,11 +751,11 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -782,11 +776,11 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="18"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -807,11 +801,11 @@
       <c r="X3" s="1"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="19"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -838,7 +832,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="5"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -857,11 +851,11 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -885,7 +879,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -907,13 +901,11 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -934,17 +926,17 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="1"/>
@@ -23784,6 +23776,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DF3CEA3A9869A24E908C80E629A011B0" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="daaeb6e23fe035e53945bf52281eec93">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4cdb0f69-8f23-4e34-9e7e-d984a4ab66dc" xmlns:ns4="6cc8bd0d-fc35-46fb-9f3e-98771e35dc48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c667dd57fcfae6b236bbf1687db50bc1" ns3:_="" ns4:_="">
     <xsd:import namespace="4cdb0f69-8f23-4e34-9e7e-d984a4ab66dc"/>
@@ -23980,7 +23978,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -23989,13 +23987,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAAFF937-1669-46D1-9A2D-83588FED2EC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6cc8bd0d-fc35-46fb-9f3e-98771e35dc48"/>
+    <ds:schemaRef ds:uri="4cdb0f69-8f23-4e34-9e7e-d984a4ab66dc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0242DE9F-656C-4C16-9824-C8E5A8871962}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24014,27 +24023,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EA9B980-7D23-417C-9DD8-F61F644C7C90}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAAFF937-1669-46D1-9A2D-83588FED2EC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6cc8bd0d-fc35-46fb-9f3e-98771e35dc48"/>
-    <ds:schemaRef ds:uri="4cdb0f69-8f23-4e34-9e7e-d984a4ab66dc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>